<commit_message>
updated with cleaning and eating time
</commit_message>
<xml_diff>
--- a/abms data.xlsx
+++ b/abms data.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Melvin ng\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Melvin ng\Desktop\ab modelling\project\ABMS-T9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EFB4D21-96FE-446B-9B10-A40981341EBF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A023C5C2-26CD-471C-B6BF-D7E52AA234CD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{AB345F5E-DDAD-4D03-BBAA-62D070B78501}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" activeTab="2" xr2:uid="{AB345F5E-DDAD-4D03-BBAA-62D070B78501}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Crowd-rate" sheetId="1" r:id="rId1"/>
+    <sheet name="Eating-time" sheetId="3" r:id="rId2"/>
+    <sheet name="Cleaning" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="34">
   <si>
     <t>Thursday</t>
   </si>
@@ -106,6 +108,33 @@
   </si>
   <si>
     <t>average observation of groups(non-peak)</t>
+  </si>
+  <si>
+    <t>Time-taken</t>
+  </si>
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>average time taken eating</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>average timing to clean a plate in seconds</t>
+  </si>
+  <si>
+    <t>Min time</t>
+  </si>
+  <si>
+    <t>Max time</t>
   </si>
 </sst>
 </file>
@@ -201,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -233,6 +262,16 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -550,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9D8ABFA-3741-43AD-9FEA-F32BEA9D2F22}">
   <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1267,4 +1306,2724 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AACF6B6-6CE3-4E92-AF70-33C3A4836986}">
+  <dimension ref="A1:G120"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="3.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.46484375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" s="17">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2">
+        <f>AVERAGE(C2:C119)</f>
+        <v>13.649572649572649</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" s="17">
+        <v>2</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3">
+        <f>MIN(C2:C119)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" s="17">
+        <v>3</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4">
+        <f>MAX(C2:C119)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" s="17">
+        <v>4</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" s="17">
+        <v>5</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" s="17">
+        <v>6</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" s="17">
+        <v>7</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9" s="17">
+        <v>8</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" s="17">
+        <v>9</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" s="17">
+        <v>10</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12" s="17">
+        <v>11</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13" s="17">
+        <v>12</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" s="17">
+        <v>13</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" s="17">
+        <v>14</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16" s="17">
+        <v>15</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" s="17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18" s="17">
+        <v>17</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A19" s="17">
+        <v>18</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A20" s="17">
+        <v>19</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A21" s="17">
+        <v>20</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A22" s="17">
+        <v>21</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A23" s="17">
+        <v>22</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A24" s="17">
+        <v>23</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A25" s="17">
+        <v>24</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A26" s="17">
+        <v>25</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A27" s="17">
+        <v>26</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A28" s="17">
+        <v>27</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A29" s="17">
+        <v>28</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A30" s="17">
+        <v>29</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A31" s="17">
+        <v>30</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A32" s="17">
+        <v>31</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A33" s="17">
+        <v>32</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A34" s="17">
+        <v>33</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A35" s="17">
+        <v>34</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A36" s="17">
+        <v>35</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A37" s="17">
+        <v>36</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A38" s="17">
+        <v>37</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A39" s="17">
+        <v>38</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A40" s="17">
+        <v>39</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A41" s="17">
+        <v>40</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A42" s="17">
+        <v>41</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A43" s="17">
+        <v>42</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A44" s="17">
+        <v>43</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A45" s="17">
+        <v>44</v>
+      </c>
+      <c r="B45" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A46" s="17">
+        <v>45</v>
+      </c>
+      <c r="B46" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A47" s="17">
+        <v>46</v>
+      </c>
+      <c r="B47" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A48" s="17">
+        <v>47</v>
+      </c>
+      <c r="B48" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A49" s="17">
+        <v>48</v>
+      </c>
+      <c r="B49" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C49">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A50" s="17">
+        <v>49</v>
+      </c>
+      <c r="B50" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C50">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A51" s="17">
+        <v>50</v>
+      </c>
+      <c r="B51" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C51">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A52" s="17">
+        <v>51</v>
+      </c>
+      <c r="B52" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C52">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A53" s="17">
+        <v>52</v>
+      </c>
+      <c r="B53" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C53">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A54" s="17">
+        <v>53</v>
+      </c>
+      <c r="B54" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C54">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A55" s="17">
+        <v>54</v>
+      </c>
+      <c r="B55" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C55">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A56" s="17">
+        <v>55</v>
+      </c>
+      <c r="B56" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C56">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A57" s="17">
+        <v>56</v>
+      </c>
+      <c r="B57" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C57">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A58" s="17">
+        <v>57</v>
+      </c>
+      <c r="B58" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C58">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A59" s="17">
+        <v>58</v>
+      </c>
+      <c r="B59" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C59">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A60" s="17">
+        <v>59</v>
+      </c>
+      <c r="B60" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C60">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A61" s="17">
+        <v>60</v>
+      </c>
+      <c r="B61" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C61">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A62" s="17">
+        <v>61</v>
+      </c>
+      <c r="B62" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C62">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A63" s="17">
+        <v>62</v>
+      </c>
+      <c r="B63" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C63">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A64" s="17">
+        <v>63</v>
+      </c>
+      <c r="B64" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C64">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A65" s="17">
+        <v>64</v>
+      </c>
+      <c r="B65" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C65">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A66" s="17">
+        <v>65</v>
+      </c>
+      <c r="B66" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C66">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A67" s="17">
+        <v>66</v>
+      </c>
+      <c r="B67" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C67">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A68" s="17">
+        <v>67</v>
+      </c>
+      <c r="B68" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C68">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A69" s="17">
+        <v>68</v>
+      </c>
+      <c r="B69" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C69">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A70" s="17">
+        <v>69</v>
+      </c>
+      <c r="B70" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C70">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A71" s="17">
+        <v>70</v>
+      </c>
+      <c r="B71" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C71">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A72" s="17">
+        <v>71</v>
+      </c>
+      <c r="B72" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C72">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A73" s="17">
+        <v>72</v>
+      </c>
+      <c r="B73" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C73">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A74" s="17">
+        <v>73</v>
+      </c>
+      <c r="B74" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C74">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A75" s="17">
+        <v>74</v>
+      </c>
+      <c r="B75" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C75">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A76" s="17">
+        <v>75</v>
+      </c>
+      <c r="B76" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C76">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A77" s="17">
+        <v>76</v>
+      </c>
+      <c r="B77" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C77">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A78" s="17">
+        <v>77</v>
+      </c>
+      <c r="B78" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C78">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A79" s="17">
+        <v>78</v>
+      </c>
+      <c r="B79" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C79">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A80" s="17">
+        <v>79</v>
+      </c>
+      <c r="B80" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C80">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A81" s="17">
+        <v>80</v>
+      </c>
+      <c r="B81" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C81">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A82" s="17">
+        <v>81</v>
+      </c>
+      <c r="B82" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C82">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A83" s="17">
+        <v>82</v>
+      </c>
+      <c r="B83" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C83">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A84" s="17">
+        <v>83</v>
+      </c>
+      <c r="B84" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C84">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A85" s="17">
+        <v>84</v>
+      </c>
+      <c r="B85" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C85">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A86" s="17">
+        <v>85</v>
+      </c>
+      <c r="B86" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C86">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A87" s="17">
+        <v>86</v>
+      </c>
+      <c r="B87" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C87">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A88" s="17">
+        <v>87</v>
+      </c>
+      <c r="B88" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C88">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A89" s="17">
+        <v>88</v>
+      </c>
+      <c r="B89" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C89">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A90" s="17">
+        <v>89</v>
+      </c>
+      <c r="B90" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C90">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A91" s="17">
+        <v>90</v>
+      </c>
+      <c r="B91" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C91">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A92" s="17">
+        <v>91</v>
+      </c>
+      <c r="B92" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C92">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A93" s="17">
+        <v>92</v>
+      </c>
+      <c r="B93" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C93">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A94" s="17">
+        <v>93</v>
+      </c>
+      <c r="B94" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C94">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A95" s="17">
+        <v>94</v>
+      </c>
+      <c r="B95" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C95">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A96" s="17">
+        <v>95</v>
+      </c>
+      <c r="B96" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C96">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A97" s="17">
+        <v>96</v>
+      </c>
+      <c r="B97" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C97">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A98" s="17">
+        <v>97</v>
+      </c>
+      <c r="B98" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C98">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A99" s="17">
+        <v>98</v>
+      </c>
+      <c r="B99" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C99">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A100" s="17">
+        <v>99</v>
+      </c>
+      <c r="B100" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C100">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A101" s="17">
+        <v>100</v>
+      </c>
+      <c r="B101" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C101">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A102" s="17">
+        <v>101</v>
+      </c>
+      <c r="B102" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C102">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A103" s="17">
+        <v>102</v>
+      </c>
+      <c r="B103" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C103">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A104" s="17">
+        <v>103</v>
+      </c>
+      <c r="B104" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C104">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A105" s="17">
+        <v>104</v>
+      </c>
+      <c r="B105" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C105">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A106" s="17">
+        <v>105</v>
+      </c>
+      <c r="B106" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C106">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A107" s="17">
+        <v>106</v>
+      </c>
+      <c r="B107" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C107">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A108" s="17">
+        <v>107</v>
+      </c>
+      <c r="B108" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C108">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A109" s="17">
+        <v>108</v>
+      </c>
+      <c r="B109" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C109">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A110" s="17">
+        <v>109</v>
+      </c>
+      <c r="B110" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C110">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A111" s="17">
+        <v>110</v>
+      </c>
+      <c r="B111" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C111">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A112" s="17">
+        <v>111</v>
+      </c>
+      <c r="B112" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C112">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A113" s="17">
+        <v>112</v>
+      </c>
+      <c r="B113" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C113">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A114" s="17">
+        <v>113</v>
+      </c>
+      <c r="B114" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C114">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A115" s="17">
+        <v>114</v>
+      </c>
+      <c r="B115" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C115">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A116" s="17">
+        <v>115</v>
+      </c>
+      <c r="B116" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C116">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A117" s="17">
+        <v>116</v>
+      </c>
+      <c r="B117" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C117">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A118" s="17">
+        <v>117</v>
+      </c>
+      <c r="B118" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C118">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A119" s="17">
+        <v>118</v>
+      </c>
+      <c r="B119" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C119">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A120" s="17">
+        <v>119</v>
+      </c>
+      <c r="B120" s="17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F21DCF71-2689-4FBB-8765-7213A580597D}">
+  <dimension ref="A1:F120"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="3.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.06640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="16">
+        <v>1</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="16">
+        <v>2</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="16">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3">
+        <f>AVERAGE(C2:C120)</f>
+        <v>12.731092436974789</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="16">
+        <v>3</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="16">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4">
+        <f>MIN(C2:C120)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="16">
+        <v>4</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="16">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5">
+        <f>MAX(C2:C120)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="16">
+        <v>5</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="16">
+        <v>6</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="16">
+        <v>7</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="16">
+        <v>8</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="16">
+        <v>9</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="16">
+        <v>10</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="16">
+        <v>11</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="16">
+        <v>12</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="16">
+        <v>13</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="16">
+        <v>14</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" s="16">
+        <v>16</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18" s="16">
+        <v>17</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A19" s="16">
+        <v>18</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A20" s="16">
+        <v>19</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A21" s="16">
+        <v>20</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A22" s="16">
+        <v>21</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A23" s="16">
+        <v>22</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A24" s="16">
+        <v>23</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A25" s="16">
+        <v>24</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A26" s="16">
+        <v>25</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A27" s="16">
+        <v>26</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A28" s="16">
+        <v>27</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A29" s="16">
+        <v>28</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A30" s="16">
+        <v>29</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A31" s="16">
+        <v>30</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A32" s="16">
+        <v>31</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A33" s="16">
+        <v>32</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A34" s="16">
+        <v>33</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A35" s="16">
+        <v>34</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A36" s="16">
+        <v>35</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A37" s="16">
+        <v>36</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A38" s="16">
+        <v>37</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A39" s="16">
+        <v>38</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" s="16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A40" s="16">
+        <v>39</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A41" s="16">
+        <v>40</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A42" s="16">
+        <v>41</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A43" s="16">
+        <v>42</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A44" s="16">
+        <v>43</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A45" s="16">
+        <v>44</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" s="16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A46" s="16">
+        <v>45</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" s="16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A47" s="16">
+        <v>46</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47" s="16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A48" s="16">
+        <v>47</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" s="16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A49" s="16">
+        <v>48</v>
+      </c>
+      <c r="B49" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C49" s="16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A50" s="16">
+        <v>49</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C50" s="16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A51" s="16">
+        <v>50</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C51" s="16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A52" s="16">
+        <v>51</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C52" s="16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A53" s="16">
+        <v>52</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C53" s="16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A54" s="16">
+        <v>53</v>
+      </c>
+      <c r="B54" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C54" s="16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A55" s="16">
+        <v>54</v>
+      </c>
+      <c r="B55" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C55" s="16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A56" s="16">
+        <v>55</v>
+      </c>
+      <c r="B56" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C56" s="16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A57" s="16">
+        <v>56</v>
+      </c>
+      <c r="B57" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C57" s="16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A58" s="16">
+        <v>57</v>
+      </c>
+      <c r="B58" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C58" s="16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A59" s="16">
+        <v>58</v>
+      </c>
+      <c r="B59" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C59" s="16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A60" s="16">
+        <v>59</v>
+      </c>
+      <c r="B60" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C60" s="16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A61" s="16">
+        <v>60</v>
+      </c>
+      <c r="B61" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C61" s="16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A62" s="16">
+        <v>61</v>
+      </c>
+      <c r="B62" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C62" s="16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A63" s="16">
+        <v>62</v>
+      </c>
+      <c r="B63" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C63" s="16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A64" s="16">
+        <v>63</v>
+      </c>
+      <c r="B64" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C64" s="16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A65" s="16">
+        <v>64</v>
+      </c>
+      <c r="B65" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C65" s="16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A66" s="16">
+        <v>65</v>
+      </c>
+      <c r="B66" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C66" s="16">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A67" s="16">
+        <v>66</v>
+      </c>
+      <c r="B67" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C67" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A68" s="16">
+        <v>67</v>
+      </c>
+      <c r="B68" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C68" s="16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A69" s="16">
+        <v>68</v>
+      </c>
+      <c r="B69" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C69" s="16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A70" s="16">
+        <v>69</v>
+      </c>
+      <c r="B70" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C70" s="16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A71" s="16">
+        <v>70</v>
+      </c>
+      <c r="B71" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C71" s="16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A72" s="16">
+        <v>71</v>
+      </c>
+      <c r="B72" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C72" s="16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A73" s="16">
+        <v>72</v>
+      </c>
+      <c r="B73" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C73" s="16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A74" s="16">
+        <v>73</v>
+      </c>
+      <c r="B74" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C74" s="16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A75" s="16">
+        <v>74</v>
+      </c>
+      <c r="B75" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C75" s="16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A76" s="16">
+        <v>75</v>
+      </c>
+      <c r="B76" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C76" s="16">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A77" s="16">
+        <v>76</v>
+      </c>
+      <c r="B77" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C77" s="16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A78" s="16">
+        <v>77</v>
+      </c>
+      <c r="B78" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C78" s="16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A79" s="16">
+        <v>78</v>
+      </c>
+      <c r="B79" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C79" s="16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A80" s="16">
+        <v>79</v>
+      </c>
+      <c r="B80" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C80" s="16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A81" s="16">
+        <v>80</v>
+      </c>
+      <c r="B81" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C81" s="16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A82" s="16">
+        <v>81</v>
+      </c>
+      <c r="B82" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C82" s="16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A83" s="16">
+        <v>82</v>
+      </c>
+      <c r="B83" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C83" s="16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A84" s="16">
+        <v>83</v>
+      </c>
+      <c r="B84" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C84" s="16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A85" s="16">
+        <v>84</v>
+      </c>
+      <c r="B85" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C85" s="16">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A86" s="16">
+        <v>85</v>
+      </c>
+      <c r="B86" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C86" s="16">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A87" s="16">
+        <v>86</v>
+      </c>
+      <c r="B87" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C87" s="16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A88" s="16">
+        <v>87</v>
+      </c>
+      <c r="B88" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C88" s="16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A89" s="16">
+        <v>88</v>
+      </c>
+      <c r="B89" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C89" s="16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A90" s="16">
+        <v>89</v>
+      </c>
+      <c r="B90" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C90" s="16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A91" s="16">
+        <v>90</v>
+      </c>
+      <c r="B91" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C91" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A92" s="16">
+        <v>91</v>
+      </c>
+      <c r="B92" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C92" s="16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A93" s="16">
+        <v>92</v>
+      </c>
+      <c r="B93" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C93" s="16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A94" s="16">
+        <v>93</v>
+      </c>
+      <c r="B94" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C94" s="16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A95" s="16">
+        <v>94</v>
+      </c>
+      <c r="B95" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C95" s="16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A96" s="16">
+        <v>95</v>
+      </c>
+      <c r="B96" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C96" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A97" s="16">
+        <v>96</v>
+      </c>
+      <c r="B97" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C97" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A98" s="16">
+        <v>97</v>
+      </c>
+      <c r="B98" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C98" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A99" s="16">
+        <v>98</v>
+      </c>
+      <c r="B99" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C99" s="16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A100" s="16">
+        <v>99</v>
+      </c>
+      <c r="B100" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C100" s="16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A101" s="16">
+        <v>100</v>
+      </c>
+      <c r="B101" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C101" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A102" s="16">
+        <v>101</v>
+      </c>
+      <c r="B102" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C102" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A103" s="16">
+        <v>102</v>
+      </c>
+      <c r="B103" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C103" s="16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A104" s="16">
+        <v>103</v>
+      </c>
+      <c r="B104" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C104" s="16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A105" s="16">
+        <v>104</v>
+      </c>
+      <c r="B105" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C105" s="16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A106" s="16">
+        <v>105</v>
+      </c>
+      <c r="B106" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C106" s="16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A107" s="16">
+        <v>106</v>
+      </c>
+      <c r="B107" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C107" s="16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A108" s="16">
+        <v>107</v>
+      </c>
+      <c r="B108" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C108" s="16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A109" s="16">
+        <v>108</v>
+      </c>
+      <c r="B109" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C109" s="16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A110" s="16">
+        <v>109</v>
+      </c>
+      <c r="B110" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C110" s="16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A111" s="16">
+        <v>110</v>
+      </c>
+      <c r="B111" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C111" s="16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A112" s="16">
+        <v>111</v>
+      </c>
+      <c r="B112" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C112" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A113" s="16">
+        <v>112</v>
+      </c>
+      <c r="B113" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C113" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A114" s="16">
+        <v>113</v>
+      </c>
+      <c r="B114" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C114" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A115" s="16">
+        <v>114</v>
+      </c>
+      <c r="B115" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C115" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A116" s="16">
+        <v>115</v>
+      </c>
+      <c r="B116" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C116" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A117" s="16">
+        <v>116</v>
+      </c>
+      <c r="B117" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C117" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A118" s="16">
+        <v>117</v>
+      </c>
+      <c r="B118" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C118" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A119" s="16">
+        <v>118</v>
+      </c>
+      <c r="B119" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C119" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A120" s="16">
+        <v>119</v>
+      </c>
+      <c r="B120" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C120" s="16">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added modification to excel
eh can add
- duration of observation for tray return
- sd of cleaning time since normal distribution right? DONE
- eating time also?  DONE
- observation for crowd-rate abit too much ah LOL DONE THOUGH
</commit_message>
<xml_diff>
--- a/abms data.xlsx
+++ b/abms data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Melvin ng\Desktop\ab modelling\project\ABMS-T9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA2C2C87-1614-4CBE-BFBA-BA0E488483C6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED01EFF-5695-409D-A061-61045AA6546A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" tabRatio="681" activeTab="3" xr2:uid="{AB345F5E-DDAD-4D03-BBAA-62D070B78501}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="45">
   <si>
     <t>Thursday</t>
   </si>
@@ -117,12 +117,6 @@
     <t>Max time</t>
   </si>
   <si>
-    <t>Trays returned</t>
-  </si>
-  <si>
-    <t>Trays unreturned</t>
-  </si>
-  <si>
     <t>Comments</t>
   </si>
   <si>
@@ -132,9 +126,6 @@
     <t>Available tray return point nearby</t>
   </si>
   <si>
-    <t xml:space="preserve">Avg  </t>
-  </si>
-  <si>
     <t>Difference in (trays returned-tray unreturned)/trays unreturned) in %</t>
   </si>
   <si>
@@ -160,6 +151,24 @@
   </si>
   <si>
     <t>Netwon Food Centre</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>Chinatown Complex Food Centre</t>
+  </si>
+  <si>
+    <t>Standard Deviation</t>
+  </si>
+  <si>
+    <t>Trays returned (in the span of 1hr)</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Trays unreturned (in the span of 1hr)</t>
   </si>
 </sst>
 </file>
@@ -621,7 +630,7 @@
   <dimension ref="A1:R28"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E10"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -749,7 +758,7 @@
         <v>545</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F4">
         <v>41</v>
@@ -805,7 +814,7 @@
         <v>612</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F5">
         <v>68</v>
@@ -838,7 +847,7 @@
         <v>612</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F6">
         <v>45</v>
@@ -871,7 +880,7 @@
         <v>701</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F7">
         <v>30</v>
@@ -904,7 +913,7 @@
         <v>624</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F8">
         <v>18</v>
@@ -937,7 +946,7 @@
         <v>712</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F9">
         <v>24</v>
@@ -970,7 +979,7 @@
         <v>921</v>
       </c>
       <c r="E10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F10">
         <v>35</v>
@@ -1075,7 +1084,7 @@
         <v>428</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F13">
         <v>48</v>
@@ -1124,7 +1133,7 @@
         <v>451</v>
       </c>
       <c r="E14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F14">
         <v>33</v>
@@ -1157,7 +1166,7 @@
         <v>601</v>
       </c>
       <c r="E15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F15">
         <v>32</v>
@@ -1190,7 +1199,7 @@
         <v>522</v>
       </c>
       <c r="E16" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F16">
         <v>50</v>
@@ -1223,7 +1232,7 @@
         <v>552</v>
       </c>
       <c r="E17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F17">
         <v>42</v>
@@ -1256,7 +1265,7 @@
         <v>700</v>
       </c>
       <c r="E18" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F18">
         <v>69</v>
@@ -1289,7 +1298,7 @@
         <v>722</v>
       </c>
       <c r="E19" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F19">
         <v>70</v>
@@ -1347,8 +1356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AACF6B6-6CE3-4E92-AF70-33C3A4836986}">
   <dimension ref="A1:G121"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B121"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1434,6 +1443,13 @@
       <c r="C5">
         <v>15</v>
       </c>
+      <c r="F5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5">
+        <f>STDEV(C2:C121)</f>
+        <v>3.6099334380888495</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="12">
@@ -1561,7 +1577,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C17">
         <v>10</v>
@@ -1572,7 +1588,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C18">
         <v>10</v>
@@ -1583,7 +1599,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C19">
         <v>12</v>
@@ -1594,7 +1610,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C20">
         <v>13</v>
@@ -1605,7 +1621,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C21">
         <v>10</v>
@@ -1616,7 +1632,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C22">
         <v>11</v>
@@ -1627,7 +1643,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C23">
         <v>13</v>
@@ -1638,7 +1654,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C24">
         <v>15</v>
@@ -1649,7 +1665,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C25">
         <v>10</v>
@@ -1660,7 +1676,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C26">
         <v>12</v>
@@ -1671,7 +1687,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C27">
         <v>13</v>
@@ -1682,7 +1698,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C28">
         <v>15</v>
@@ -1693,7 +1709,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C29">
         <v>11</v>
@@ -1704,7 +1720,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C30">
         <v>13</v>
@@ -1715,7 +1731,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C31">
         <v>17</v>
@@ -1726,7 +1742,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C32">
         <v>12</v>
@@ -1737,7 +1753,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C33">
         <v>17</v>
@@ -1748,7 +1764,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C34">
         <v>15</v>
@@ -1759,7 +1775,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C35">
         <v>14</v>
@@ -1770,7 +1786,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C36">
         <v>13</v>
@@ -1781,7 +1797,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C37">
         <v>12</v>
@@ -1792,7 +1808,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C38">
         <v>17</v>
@@ -1803,7 +1819,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C39">
         <v>12</v>
@@ -1814,7 +1830,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C40">
         <v>16</v>
@@ -1825,7 +1841,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C41">
         <v>17</v>
@@ -1836,7 +1852,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C42">
         <v>12</v>
@@ -1847,7 +1863,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C43">
         <v>16</v>
@@ -1858,7 +1874,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C44">
         <v>16</v>
@@ -1869,7 +1885,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C45">
         <v>17</v>
@@ -1880,7 +1896,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C46" t="s">
         <v>20</v>
@@ -1891,7 +1907,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C47">
         <v>17</v>
@@ -1902,7 +1918,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C48">
         <v>18</v>
@@ -1913,7 +1929,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C49">
         <v>20</v>
@@ -1924,7 +1940,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C50">
         <v>19</v>
@@ -1935,7 +1951,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C51">
         <v>19</v>
@@ -1946,7 +1962,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C52">
         <v>18</v>
@@ -1957,7 +1973,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C53">
         <v>21</v>
@@ -1968,7 +1984,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C54">
         <v>16</v>
@@ -1979,7 +1995,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C55">
         <v>20</v>
@@ -1990,7 +2006,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C56">
         <v>19</v>
@@ -2001,7 +2017,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C57">
         <v>20</v>
@@ -2012,7 +2028,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C58">
         <v>20</v>
@@ -2023,7 +2039,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C59">
         <v>16</v>
@@ -2034,7 +2050,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C60">
         <v>16</v>
@@ -2045,7 +2061,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C61">
         <v>11</v>
@@ -2056,7 +2072,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C62">
         <v>14</v>
@@ -2067,7 +2083,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C63">
         <v>12</v>
@@ -2078,7 +2094,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C64">
         <v>14</v>
@@ -2089,7 +2105,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C65">
         <v>11</v>
@@ -2100,7 +2116,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C66">
         <v>12</v>
@@ -2111,7 +2127,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C67">
         <v>10</v>
@@ -2122,7 +2138,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C68">
         <v>14</v>
@@ -2133,7 +2149,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C69">
         <v>13</v>
@@ -2144,7 +2160,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C70">
         <v>12</v>
@@ -2155,7 +2171,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C71">
         <v>13</v>
@@ -2166,7 +2182,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C72">
         <v>11</v>
@@ -2177,7 +2193,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C73">
         <v>10</v>
@@ -2188,7 +2204,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C74">
         <v>10</v>
@@ -2199,7 +2215,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C75">
         <v>12</v>
@@ -2210,7 +2226,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C76">
         <v>9</v>
@@ -2221,7 +2237,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C77">
         <v>12</v>
@@ -2232,7 +2248,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C78">
         <v>8</v>
@@ -2243,7 +2259,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C79">
         <v>10</v>
@@ -2254,7 +2270,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C80">
         <v>10</v>
@@ -2265,7 +2281,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C81">
         <v>9</v>
@@ -2276,7 +2292,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C82">
         <v>9</v>
@@ -2287,7 +2303,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C83">
         <v>9</v>
@@ -2298,7 +2314,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C84">
         <v>10</v>
@@ -2309,7 +2325,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C85">
         <v>8</v>
@@ -2320,7 +2336,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C86">
         <v>11</v>
@@ -2331,7 +2347,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C87">
         <v>9</v>
@@ -2342,7 +2358,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C88">
         <v>12</v>
@@ -2353,7 +2369,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C89">
         <v>8</v>
@@ -2364,7 +2380,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C90">
         <v>8</v>
@@ -2375,7 +2391,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C91">
         <v>12</v>
@@ -2386,7 +2402,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C92">
         <v>10</v>
@@ -2397,7 +2413,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C93">
         <v>13</v>
@@ -2408,7 +2424,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C94">
         <v>10</v>
@@ -2419,7 +2435,7 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C95">
         <v>12</v>
@@ -2430,7 +2446,7 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C96">
         <v>12</v>
@@ -2441,7 +2457,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C97">
         <v>10</v>
@@ -2452,7 +2468,7 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C98">
         <v>11</v>
@@ -2463,7 +2479,7 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C99">
         <v>12</v>
@@ -2474,7 +2490,7 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C100">
         <v>12</v>
@@ -2485,7 +2501,7 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C101">
         <v>13</v>
@@ -2496,7 +2512,7 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C102">
         <v>11</v>
@@ -2507,7 +2523,7 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C103">
         <v>10</v>
@@ -2518,7 +2534,7 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C104">
         <v>11</v>
@@ -2529,7 +2545,7 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C105">
         <v>12</v>
@@ -2540,7 +2556,7 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C106">
         <v>14</v>
@@ -2551,7 +2567,7 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C107">
         <v>11</v>
@@ -2562,7 +2578,7 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C108">
         <v>12</v>
@@ -2573,7 +2589,7 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C109">
         <v>13</v>
@@ -2584,7 +2600,7 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C110">
         <v>15</v>
@@ -2595,7 +2611,7 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C111">
         <v>11</v>
@@ -2606,7 +2622,7 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C112">
         <v>14</v>
@@ -2617,7 +2633,7 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C113">
         <v>12</v>
@@ -2628,7 +2644,7 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C114">
         <v>14</v>
@@ -2639,7 +2655,7 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C115">
         <v>15</v>
@@ -2650,7 +2666,7 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C116">
         <v>11</v>
@@ -2661,7 +2677,7 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C117">
         <v>12</v>
@@ -2672,7 +2688,7 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C118">
         <v>11</v>
@@ -2683,7 +2699,7 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C119">
         <v>15</v>
@@ -2694,7 +2710,7 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C120">
         <v>13</v>
@@ -2702,7 +2718,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B121" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C121">
         <v>12</v>
@@ -2722,12 +2738,12 @@
   <dimension ref="A1:F121"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B121"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="3.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.3984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.06640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -2818,6 +2834,13 @@
       <c r="C6" s="11">
         <v>13</v>
       </c>
+      <c r="E6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6">
+        <f>STDEV(C2:C121)</f>
+        <v>2.7743826123214919</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="11">
@@ -2934,7 +2957,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C17" s="11">
         <v>9</v>
@@ -2945,7 +2968,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C18" s="11">
         <v>8</v>
@@ -2956,7 +2979,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C19" s="11">
         <v>13</v>
@@ -2967,7 +2990,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C20" s="11">
         <v>10</v>
@@ -2978,7 +3001,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C21" s="11">
         <v>13</v>
@@ -2989,7 +3012,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C22" s="11">
         <v>8</v>
@@ -3000,7 +3023,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C23" s="11">
         <v>9</v>
@@ -3011,7 +3034,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C24" s="11">
         <v>13</v>
@@ -3022,7 +3045,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C25" s="11">
         <v>8</v>
@@ -3033,7 +3056,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C26" s="11">
         <v>9</v>
@@ -3044,7 +3067,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C27" s="11">
         <v>9</v>
@@ -3055,7 +3078,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C28" s="11">
         <v>8</v>
@@ -3066,7 +3089,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C29" s="11">
         <v>13</v>
@@ -3077,7 +3100,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C30" s="11">
         <v>12</v>
@@ -3088,7 +3111,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C31" s="11">
         <v>9</v>
@@ -3099,7 +3122,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C32" s="11">
         <v>9</v>
@@ -3110,7 +3133,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C33" s="11">
         <v>13</v>
@@ -3121,7 +3144,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C34" s="11">
         <v>12</v>
@@ -3132,7 +3155,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C35" s="11">
         <v>13</v>
@@ -3143,7 +3166,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C36" s="11">
         <v>11</v>
@@ -3154,7 +3177,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C37" s="11">
         <v>13</v>
@@ -3165,7 +3188,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C38" s="11">
         <v>11</v>
@@ -3176,7 +3199,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C39" s="11">
         <v>12</v>
@@ -3187,7 +3210,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C40" s="11">
         <v>9</v>
@@ -3198,7 +3221,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C41" s="11">
         <v>11</v>
@@ -3209,7 +3232,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C42" s="11">
         <v>13</v>
@@ -3220,7 +3243,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C43" s="11">
         <v>8</v>
@@ -3231,7 +3254,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C44" s="11">
         <v>13</v>
@@ -3242,7 +3265,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C45" s="11">
         <v>9</v>
@@ -3253,7 +3276,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C46" s="11">
         <v>9</v>
@@ -3264,7 +3287,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C47" s="11">
         <v>14</v>
@@ -3275,7 +3298,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C48" s="11">
         <v>11</v>
@@ -3286,7 +3309,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C49" s="11">
         <v>11</v>
@@ -3297,7 +3320,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C50" s="11">
         <v>9</v>
@@ -3308,7 +3331,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C51" s="11">
         <v>14</v>
@@ -3319,7 +3342,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C52" s="11">
         <v>11</v>
@@ -3330,7 +3353,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C53" s="11">
         <v>12</v>
@@ -3341,7 +3364,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C54" s="11">
         <v>11</v>
@@ -3352,7 +3375,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C55" s="11">
         <v>12</v>
@@ -3363,7 +3386,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C56" s="11">
         <v>10</v>
@@ -3374,7 +3397,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C57" s="11">
         <v>12</v>
@@ -3385,7 +3408,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C58" s="11">
         <v>9</v>
@@ -3396,7 +3419,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C59" s="11">
         <v>9</v>
@@ -3407,7 +3430,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C60" s="11">
         <v>11</v>
@@ -3418,7 +3441,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C61" s="11">
         <v>12</v>
@@ -3429,7 +3452,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C62" s="11">
         <v>14</v>
@@ -3440,7 +3463,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C63" s="11">
         <v>14</v>
@@ -3451,7 +3474,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C64" s="11">
         <v>15</v>
@@ -3462,7 +3485,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C65" s="11">
         <v>10</v>
@@ -3473,7 +3496,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C66" s="11">
         <v>18</v>
@@ -3484,7 +3507,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C67" s="11">
         <v>13</v>
@@ -3495,7 +3518,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C68" s="11">
         <v>14</v>
@@ -3506,7 +3529,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C69" s="11">
         <v>14</v>
@@ -3517,7 +3540,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C70" s="11">
         <v>14</v>
@@ -3528,7 +3551,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C71" s="11">
         <v>11</v>
@@ -3539,7 +3562,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C72" s="11">
         <v>20</v>
@@ -3550,7 +3573,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C73" s="11">
         <v>20</v>
@@ -3561,7 +3584,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C74" s="11">
         <v>11</v>
@@ -3572,7 +3595,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C75" s="11">
         <v>15</v>
@@ -3583,7 +3606,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C76" s="11">
         <v>19</v>
@@ -3594,7 +3617,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C77" s="11">
         <v>16</v>
@@ -3605,7 +3628,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C78" s="11">
         <v>16</v>
@@ -3616,7 +3639,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C79" s="11">
         <v>16</v>
@@ -3627,7 +3650,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C80" s="11">
         <v>10</v>
@@ -3638,7 +3661,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C81" s="11">
         <v>12</v>
@@ -3649,7 +3672,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C82" s="11">
         <v>20</v>
@@ -3660,7 +3683,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C83" s="11">
         <v>16</v>
@@ -3671,7 +3694,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C84" s="11">
         <v>20</v>
@@ -3682,7 +3705,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C85" s="11">
         <v>19</v>
@@ -3693,7 +3716,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C86" s="11">
         <v>18</v>
@@ -3704,7 +3727,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C87" s="11">
         <v>20</v>
@@ -3715,7 +3738,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C88" s="11">
         <v>16</v>
@@ -3726,7 +3749,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C89" s="11">
         <v>16</v>
@@ -3737,7 +3760,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C90" s="11">
         <v>16</v>
@@ -3748,7 +3771,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C91" s="11">
         <v>13</v>
@@ -3759,7 +3782,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C92" s="11">
         <v>15</v>
@@ -3770,7 +3793,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C93" s="11">
         <v>11</v>
@@ -3781,7 +3804,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C94" s="11">
         <v>15</v>
@@ -3792,7 +3815,7 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C95" s="11">
         <v>14</v>
@@ -3803,7 +3826,7 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C96" s="11">
         <v>13</v>
@@ -3814,7 +3837,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C97" s="11">
         <v>13</v>
@@ -3825,7 +3848,7 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C98" s="11">
         <v>13</v>
@@ -3836,7 +3859,7 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C99" s="11">
         <v>14</v>
@@ -3847,7 +3870,7 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C100" s="11">
         <v>12</v>
@@ -3858,7 +3881,7 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C101" s="11">
         <v>13</v>
@@ -3869,7 +3892,7 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C102" s="11">
         <v>13</v>
@@ -3880,7 +3903,7 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C103" s="11">
         <v>10</v>
@@ -3891,7 +3914,7 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C104" s="11">
         <v>11</v>
@@ -3902,7 +3925,7 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C105" s="11">
         <v>12</v>
@@ -3913,7 +3936,7 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C106" s="11">
         <v>12</v>
@@ -3924,7 +3947,7 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C107" s="11">
         <v>11</v>
@@ -3935,7 +3958,7 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C108" s="11">
         <v>14</v>
@@ -3946,7 +3969,7 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C109" s="11">
         <v>12</v>
@@ -3957,7 +3980,7 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C110" s="11">
         <v>12</v>
@@ -3968,7 +3991,7 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C111" s="11">
         <v>14</v>
@@ -3979,7 +4002,7 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C112" s="11">
         <v>12</v>
@@ -3990,7 +4013,7 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C113" s="11">
         <v>13</v>
@@ -4001,7 +4024,7 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C114" s="11">
         <v>13</v>
@@ -4012,7 +4035,7 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C115" s="11">
         <v>13</v>
@@ -4023,7 +4046,7 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C116" s="11">
         <v>13</v>
@@ -4034,7 +4057,7 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C117" s="11">
         <v>13</v>
@@ -4045,7 +4068,7 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C118" s="11">
         <v>11</v>
@@ -4056,7 +4079,7 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C119" s="11">
         <v>13</v>
@@ -4067,15 +4090,18 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C120" s="11">
         <v>12</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A121" s="11">
+        <v>120</v>
+      </c>
       <c r="B121" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C121" s="11">
         <v>12</v>
@@ -4084,7 +4110,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B17" r:id="rId1" tooltip="Chinatown Complex Food Centre" display="https://www.thebestsingapore.com/best-place/chinatown-complex-food-centre/" xr:uid="{5AFEAB6D-5DE4-467D-AF23-C0BB2995E1A7}"/>
-    <hyperlink ref="B18:B31" r:id="rId2" tooltip="Chinatown Complex Food Centre" display="https://www.thebestsingapore.com/best-place/chinatown-complex-food-centre/" xr:uid="{85366EC9-AD43-4C12-B4C8-AB27B0C69E1D}"/>
+    <hyperlink ref="B18:B31" r:id="rId2" tooltip="Chinatown Complex Food Centre" display="https://www.thebestsingapore.com/best-place/chinatown-complex-food-centre/" xr:uid="{E4EA798C-E900-4E5E-A111-F5130CC4B237}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4095,13 +4121,13 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="32.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.9296875" customWidth="1"/>
     <col min="5" max="5" width="18.86328125" customWidth="1"/>
@@ -4113,20 +4139,20 @@
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
@@ -4148,25 +4174,25 @@
         <v>50</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="I2" s="11">
         <f>SUM(E2:E9)/8</f>
-        <v>73.01136363636364</v>
+        <v>43.844696969696969</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B3" s="11">
+        <v>10</v>
+      </c>
+      <c r="C3" s="11">
         <v>20</v>
-      </c>
-      <c r="C3" s="11">
-        <v>10</v>
       </c>
       <c r="D3" s="11">
         <f t="shared" ref="D3:D9" si="0">SUM(B3:C3)</f>
@@ -4174,7 +4200,7 @@
       </c>
       <c r="E3" s="11">
         <f t="shared" ref="E3:E9" si="1">(B3-C3)/(C3)*100</f>
-        <v>100</v>
+        <v>-50</v>
       </c>
       <c r="F3" s="14" t="s">
         <v>31</v>
@@ -4182,7 +4208,7 @@
     </row>
     <row r="4" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B4" s="11">
         <v>19</v>
@@ -4199,12 +4225,12 @@
         <v>72.727272727272734</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B5" s="11">
         <v>8</v>
@@ -4221,12 +4247,12 @@
         <v>-63.636363636363633</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B6" s="11">
         <v>20</v>
@@ -4243,18 +4269,18 @@
         <v>100</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B7" s="11">
+        <v>12</v>
+      </c>
+      <c r="C7" s="11">
         <v>18</v>
-      </c>
-      <c r="C7" s="11">
-        <v>12</v>
       </c>
       <c r="D7" s="11">
         <f t="shared" si="0"/>
@@ -4262,7 +4288,7 @@
       </c>
       <c r="E7" s="11">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>-33.333333333333329</v>
       </c>
       <c r="F7" s="14" t="s">
         <v>31</v>
@@ -4270,7 +4296,7 @@
     </row>
     <row r="8" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B8" s="11">
         <v>20</v>
@@ -4287,12 +4313,12 @@
         <v>100</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B9" s="11">
         <v>22</v>
@@ -4309,7 +4335,7 @@
         <v>175</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>